<commit_message>
Adding ID and TRT info
</commit_message>
<xml_diff>
--- a/Data/2018-07-31_Trikinetic_workbook.xlsx
+++ b/Data/2018-07-31_Trikinetic_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtussey\Desktop\Aedes-aegypti-Anoxia-Irradiation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FA886E-2801-4BAE-8231-B01DDFE74CA0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19591825-311B-4A2C-9CFC-D20C7C1B9056}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" xr2:uid="{1CA2E361-8382-4FF0-906C-BC1512380B2F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Cohort_Date</t>
   </si>
@@ -61,6 +61,102 @@
   </si>
   <si>
     <t>Time_Out_Hour</t>
+  </si>
+  <si>
+    <t>x018</t>
+  </si>
+  <si>
+    <t>x028</t>
+  </si>
+  <si>
+    <t>x008</t>
+  </si>
+  <si>
+    <t>x030</t>
+  </si>
+  <si>
+    <t>x003</t>
+  </si>
+  <si>
+    <t>x009</t>
+  </si>
+  <si>
+    <t>x025</t>
+  </si>
+  <si>
+    <t>x016</t>
+  </si>
+  <si>
+    <t>x021</t>
+  </si>
+  <si>
+    <t>x023</t>
+  </si>
+  <si>
+    <t>x005</t>
+  </si>
+  <si>
+    <t>x020</t>
+  </si>
+  <si>
+    <t>x013</t>
+  </si>
+  <si>
+    <t>x012</t>
+  </si>
+  <si>
+    <t>x032</t>
+  </si>
+  <si>
+    <t>x002</t>
+  </si>
+  <si>
+    <t>x026</t>
+  </si>
+  <si>
+    <t>x014</t>
+  </si>
+  <si>
+    <t>x029</t>
+  </si>
+  <si>
+    <t>x015</t>
+  </si>
+  <si>
+    <t>x031</t>
+  </si>
+  <si>
+    <t>x004</t>
+  </si>
+  <si>
+    <t>x024</t>
+  </si>
+  <si>
+    <t>x006</t>
+  </si>
+  <si>
+    <t>x010</t>
+  </si>
+  <si>
+    <t>x017</t>
+  </si>
+  <si>
+    <t>x007</t>
+  </si>
+  <si>
+    <t>x001</t>
+  </si>
+  <si>
+    <t>x027</t>
+  </si>
+  <si>
+    <t>x022</t>
+  </si>
+  <si>
+    <t>x011</t>
+  </si>
+  <si>
+    <t>x019</t>
   </si>
 </sst>
 </file>
@@ -96,9 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,16 +512,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC654E4F-1836-487E-80D7-322CAD9E7EEF}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -434,10 +534,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" t="s">
@@ -469,8 +569,740 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="4">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>50</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>100</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4">
+        <v>100</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4">
+        <v>100</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4">
+        <v>50</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>50</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="G20" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4">
+        <v>100</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4">
+        <v>50</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4">
+        <v>50</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+      <c r="G24" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4">
+        <v>100</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4">
+        <v>50</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>27</v>
+      </c>
+      <c r="G28" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4">
+        <v>100</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
+      </c>
+      <c r="G29" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4">
+        <v>100</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="4">
+        <v>20</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>31</v>
+      </c>
+      <c r="G32" s="2">
+        <v>43312</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4">
+        <v>20</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33" s="2">
+        <v>43312</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>